<commit_message>
Atualizando o backlog e a modelagem
</commit_message>
<xml_diff>
--- a/BackLog/MetodologiasEBackLog-GR05.xlsx
+++ b/BackLog/MetodologiasEBackLog-GR05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/249c92f571d57ca1/Área de Trabalho/sprint2/Moum-Soya/BackLog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{0DC12159-227E-4C0B-A503-7B4B9320355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFD07A3B-FFD2-438B-8518-2457CB79B146}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{0DC12159-227E-4C0B-A503-7B4B9320355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{503DE509-444D-45C0-B0F8-4B975044B397}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2415,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="91" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="91" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3332,8 +3332,8 @@
       <c r="I26" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J26" s="9" t="s">
-        <v>77</v>
+      <c r="J26" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
@@ -3364,8 +3364,8 @@
       <c r="I27" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="J27" s="9" t="s">
-        <v>77</v>
+      <c r="J27" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3396,8 +3396,8 @@
       <c r="I28" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J28" s="9" t="s">
-        <v>77</v>
+      <c r="J28" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4036,8 +4036,8 @@
       <c r="I48" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="J48" s="10" t="s">
-        <v>81</v>
+      <c r="J48" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
@@ -4164,8 +4164,8 @@
       <c r="I52" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="J52" s="10" t="s">
-        <v>81</v>
+      <c r="J52" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4228,8 +4228,8 @@
       <c r="I54" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J54" s="10" t="s">
-        <v>81</v>
+      <c r="J54" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
@@ -4260,8 +4260,8 @@
       <c r="I55" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="J55" s="10" t="s">
-        <v>81</v>
+      <c r="J55" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
@@ -4292,8 +4292,8 @@
       <c r="I56" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="J56" s="10" t="s">
-        <v>81</v>
+      <c r="J56" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -4437,12 +4437,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD11765F9AC0004AAF0A4CAAFDFAF16A" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1cc742c03ab36aa87466a9c68feca297">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9fdc8751-6fef-42ec-b05c-835dd8c535b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7a3de26cefa8042fb80bd6689b2d941" ns3:_="">
     <xsd:import namespace="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
@@ -4592,6 +4586,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4602,22 +4602,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38D996E2-2738-449B-ADA8-E6769880D412}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD12F661-93DF-41F2-B906-EE9B8965009D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4635,6 +4619,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38D996E2-2738-449B-ADA8-E6769880D412}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9fdc8751-6fef-42ec-b05c-835dd8c535b4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C884185-1C22-44A8-BD74-F9D8A0E207E0}">
   <ds:schemaRefs>

</xml_diff>